<commit_message>
Created Basic Trading Algorithm Seperate From AI
</commit_message>
<xml_diff>
--- a/Completed Projects/Bitcoin Miner Data Collector/Data - ASICs.xlsx
+++ b/Completed Projects/Bitcoin Miner Data Collector/Data - ASICs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,987 +488,987 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Baikal Giant+</t>
+          <t>BITFURY B8</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>0.32</v>
+        <v>13.21</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>3.19</v>
+        <v>94.90000000000001</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>10.71</v>
+        <v>463.31</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>2.89</v>
+        <v>39.52</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>20.23</v>
+        <v>279.14</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>86.69</v>
+        <v>1196.42</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>-2.57</v>
+        <v>-26.31</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>-17.04</v>
+        <v>-184.24</v>
       </c>
       <c r="J2" t="n">
-        <v>-75.98</v>
+        <v>-733.11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Baikal Giant B</t>
+          <t>BITMAIN AntMiner D3</t>
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>2.63</v>
+        <v>0.55</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>17.7</v>
+        <v>4.52</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>79.38</v>
+        <v>17.14</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>2.12</v>
+        <v>7.49</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>14.86</v>
+        <v>52.42</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>63.71</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>2.84</v>
+        <v>224.41</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>-6.94</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>-47.89</v>
       </c>
       <c r="J3" t="n">
-        <v>15.68</v>
+        <v>-207.27</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Baikal Giant X10</t>
+          <t>BITMAIN AntMiner D5</t>
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.98</v>
+        <v>4.38</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>7.06</v>
+        <v>35.89</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>36.86</v>
+        <v>135.95</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>4.37</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>30.58</v>
+        <v>67.97</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>131.04</v>
+        <v>290.98</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>-3.39</v>
+        <v>-5.33</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>-23.52</v>
+        <v>-32.08</v>
       </c>
       <c r="J4" t="n">
-        <v>-94.18000000000001</v>
+        <v>-155.03</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BITFURY B8</t>
+          <t>BITMAIN AntMiner K5</t>
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>13.08</v>
+        <v>6.25</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>93.01000000000001</v>
+        <v>43.36</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>403.66</v>
+        <v>163.11</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>43.01</v>
+        <v>9.76</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>301.06</v>
+        <v>68.91</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>1290.24</v>
+        <v>295.37</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>-29.93</v>
+        <v>-3.5</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>-208.04</v>
+        <v>-25.55</v>
       </c>
       <c r="J5" t="n">
-        <v>-886.58</v>
+        <v>-132.25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner D3</t>
+          <t>BITMAIN AntMiner L3 ++</t>
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.28</v>
+        <v>14.77</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>1.99</v>
+        <v>99.25</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>9.789999999999999</v>
+        <v>342.74</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>8.06</v>
+        <v>6.55</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>56.45</v>
+        <v>45.86</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>241.92</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>-7.79</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>-54.46</v>
+        <v>196.36</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>8.220000000000001</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>53.38</v>
       </c>
       <c r="J6" t="n">
-        <v>-232.13</v>
+        <v>146.39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner D5</t>
+          <t>BITMAIN AntMiner L3+</t>
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>2.19</v>
+        <v>12.39</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>15.79</v>
+        <v>83.81999999999999</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>77.63</v>
+        <v>289.73</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>10.35</v>
+        <v>4.94</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>73.09</v>
+        <v>34.89</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>313.58</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>-8.16</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>-57.29</v>
+        <v>149.55</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>7.45</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>48.93</v>
       </c>
       <c r="J7" t="n">
-        <v>-235.95</v>
+        <v>140.18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner L3 ++</t>
+          <t>BITMAIN AntMiner S11</t>
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>3.06</v>
+        <v>5.57</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>21.98</v>
+        <v>39.16</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>92.94</v>
+        <v>190.92</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>7.06</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>49.39</v>
+        <v>66.83</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>211.68</v>
+        <v>286.12</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>-4</v>
+        <v>-3.98</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>-27.41</v>
+        <v>-27.67</v>
       </c>
       <c r="J8" t="n">
-        <v>-118.74</v>
+        <v>-95.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner L3+</t>
+          <t>BITMAIN AntMiner S15</t>
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>2.58</v>
+        <v>7.6</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>18.59</v>
+        <v>53.48</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>78.59999999999999</v>
+        <v>260.77</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>5.38</v>
+        <v>9.960000000000001</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>37.63</v>
+        <v>69.70999999999999</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>161.28</v>
+        <v>298.46</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>-2.79</v>
+        <v>-2.35</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>-19.05</v>
+        <v>-16.23</v>
       </c>
       <c r="J9" t="n">
-        <v>-82.68000000000001</v>
+        <v>-37.69</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S11</t>
+          <t>BITMAIN AntMiner S17</t>
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>5.36</v>
+        <v>23.09</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>38.15</v>
+        <v>162.36</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>165.58</v>
+        <v>791.62</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>10.28</v>
+        <v>14.88</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>71.97</v>
+        <v>104.18</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>308.45</v>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>-4.92</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>-33.83</v>
+        <v>446.01</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>58.19</v>
       </c>
       <c r="J10" t="n">
-        <v>-142.87</v>
+        <v>345.62</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S15</t>
+          <t>BITMAIN AntMiner S17 Pro</t>
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>7.32</v>
+        <v>23.08</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>52.1</v>
+        <v>161.92</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>226.16</v>
+        <v>788.52</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>10.73</v>
+        <v>12.32</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>75.08</v>
+        <v>86.27</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>321.75</v>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>-3.4</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>-22.97</v>
+        <v>369.33</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>10.76</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>75.65000000000001</v>
       </c>
       <c r="J11" t="n">
-        <v>-95.59</v>
+        <v>419.19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S17</t>
+          <t>BITMAIN AntMiner S17+</t>
         </is>
       </c>
       <c r="B12" s="1" t="n">
-        <v>22.23</v>
+        <v>21.73</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>158.17</v>
+        <v>152.81</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>686.55</v>
+        <v>745.0599999999999</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>16.03</v>
+        <v>18.22</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>112.19</v>
+        <v>127.55</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>480.82</v>
+        <v>546.05</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>6.2</v>
+        <v>3.51</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>45.98</v>
+        <v>25.27</v>
       </c>
       <c r="J12" t="n">
-        <v>205.74</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S17+</t>
+          <t>BITMAIN AntMiner S19</t>
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>20.92</v>
+        <v>25.79</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>148.86</v>
+        <v>180.87</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>646.17</v>
+        <v>878.35</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>19.62</v>
+        <v>20.28</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>137.36</v>
+        <v>141.96</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>588.67</v>
+        <v>607.77</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>1.3</v>
+        <v>5.51</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>11.51</v>
+        <v>38.91</v>
       </c>
       <c r="J13" t="n">
-        <v>57.5</v>
+        <v>270.59</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S17e (64Th)</t>
+          <t>BITMAIN AntMiner S19</t>
         </is>
       </c>
       <c r="B14" s="1" t="n">
-        <v>16.22</v>
+        <v>25.37</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>116.99</v>
+        <v>180.57</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>490.94</v>
+        <v>880.55</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>19.15</v>
+        <v>20.28</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>135.27</v>
+        <v>141.96</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>580.41</v>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>-2.93</v>
-      </c>
-      <c r="I14" s="2" t="n">
-        <v>-18.28</v>
+        <v>607.77</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>38.61</v>
       </c>
       <c r="J14" t="n">
-        <v>-89.47</v>
+        <v>272.79</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S17 Pro</t>
+          <t>BITMAIN AntMiner S19 Pro</t>
         </is>
       </c>
       <c r="B15" s="1" t="n">
-        <v>22.23</v>
+        <v>29.38</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>158.17</v>
+        <v>209.08</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>686.55</v>
+        <v>1019.59</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>13.27</v>
+        <v>20.28</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>92.90000000000001</v>
+        <v>141.96</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>398.16</v>
+        <v>607.77</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>8.960000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>65.26000000000001</v>
+        <v>67.12</v>
       </c>
       <c r="J15" t="n">
-        <v>288.39</v>
+        <v>411.82</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S19</t>
+          <t>BITMAIN AntMiner S19 Pro</t>
         </is>
       </c>
       <c r="B16" s="1" t="n">
-        <v>24.08</v>
+        <v>29.87</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>173.66</v>
+        <v>209.43</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>728.73</v>
+        <v>1017.04</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>21.61</v>
+        <v>20.28</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>152.65</v>
+        <v>141.96</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>654.97</v>
+        <v>607.77</v>
       </c>
       <c r="H16" s="1" t="n">
-        <v>2.47</v>
+        <v>9.59</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>21.01</v>
+        <v>67.47</v>
       </c>
       <c r="J16" t="n">
-        <v>73.76000000000001</v>
+        <v>409.27</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S19</t>
+          <t>BITMAIN AntMiner S9</t>
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>24.84</v>
+        <v>4.35</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>176.73</v>
+        <v>30.56</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>766.96</v>
+        <v>149.01</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>21.84</v>
+        <v>7.03</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>152.88</v>
+        <v>49.23</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>655.2</v>
-      </c>
-      <c r="H17" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="I17" s="1" t="n">
-        <v>23.85</v>
+        <v>210.75</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>-2.69</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>-18.67</v>
       </c>
       <c r="J17" t="n">
-        <v>111.76</v>
+        <v>-61.74</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S19 Pro</t>
+          <t>BITMAIN AntMiner S9 SE</t>
         </is>
       </c>
       <c r="B18" s="1" t="n">
-        <v>28.77</v>
+        <v>4.27</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>204.63</v>
+        <v>30.41</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>888.0599999999999</v>
+        <v>148.3</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>21.84</v>
+        <v>7.99</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>152.88</v>
+        <v>55.91</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>655.2</v>
-      </c>
-      <c r="H18" s="1" t="n">
-        <v>6.93</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>51.75</v>
+        <v>239.37</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>-3.71</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>-25.5</v>
       </c>
       <c r="J18" t="n">
-        <v>232.86</v>
+        <v>-91.06</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S19 Pro</t>
+          <t>BITMAIN AntMiner S9i</t>
         </is>
       </c>
       <c r="B19" s="1" t="n">
-        <v>27.88</v>
+        <v>4.35</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>201.08</v>
+        <v>30.56</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>843.8</v>
+        <v>149.01</v>
       </c>
       <c r="E19" s="1" t="n">
-        <v>21.61</v>
+        <v>8.24</v>
       </c>
       <c r="F19" s="1" t="n">
-        <v>152.65</v>
+        <v>57.66</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>654.97</v>
-      </c>
-      <c r="H19" s="1" t="n">
-        <v>6.27</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <v>48.43</v>
+        <v>246.85</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>-3.89</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>-27.1</v>
       </c>
       <c r="J19" t="n">
-        <v>188.82</v>
+        <v>-97.84</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S9</t>
+          <t>BITMAIN AntMiner S9j</t>
         </is>
       </c>
       <c r="B20" s="1" t="n">
-        <v>4.18</v>
+        <v>4.35</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>29.77</v>
+        <v>30.56</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>129.23</v>
+        <v>149.01</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>7.57</v>
+        <v>8.42</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>53.01</v>
+        <v>58.97</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>227.2</v>
+        <v>252.46</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>-3.39</v>
+        <v>-4.08</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>-23.24</v>
+        <v>-28.41</v>
       </c>
       <c r="J20" t="n">
-        <v>-97.97</v>
+        <v>-103.45</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S9i</t>
+          <t>BITMAIN AntMiner S9k</t>
         </is>
       </c>
       <c r="B21" s="1" t="n">
-        <v>4.18</v>
+        <v>4.35</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>29.77</v>
+        <v>30.56</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>129.23</v>
+        <v>149.01</v>
       </c>
       <c r="E21" s="1" t="n">
-        <v>8.869999999999999</v>
+        <v>8.17</v>
       </c>
       <c r="F21" s="1" t="n">
-        <v>62.09</v>
+        <v>57.22</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>266.11</v>
+        <v>244.98</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>-4.69</v>
+        <v>-3.83</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>-32.32</v>
+        <v>-26.66</v>
       </c>
       <c r="J21" t="n">
-        <v>-136.88</v>
+        <v>-95.97</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S9j</t>
+          <t>BITMAIN AntMiner T15</t>
         </is>
       </c>
       <c r="B22" s="1" t="n">
-        <v>4.18</v>
+        <v>6.25</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>29.77</v>
+        <v>43.79</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>129.23</v>
+        <v>212.65</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>9.07</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="F22" s="1" t="n">
-        <v>63.5</v>
+        <v>67.27</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>272.16</v>
+        <v>287.99</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>-4.89</v>
+        <v>-3.36</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>-33.73</v>
+        <v>-23.48</v>
       </c>
       <c r="J22" t="n">
-        <v>-142.93</v>
+        <v>-75.33</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S9k</t>
+          <t>BITMAIN AntMiner T17</t>
         </is>
       </c>
       <c r="B23" s="1" t="n">
-        <v>4.18</v>
+        <v>16.3</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>29.77</v>
+        <v>114.61</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>129.23</v>
+        <v>558.79</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>8.800000000000001</v>
+        <v>13.73</v>
       </c>
       <c r="F23" s="1" t="n">
-        <v>61.62</v>
+        <v>96.09999999999999</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>264.1</v>
-      </c>
-      <c r="H23" s="2" t="n">
-        <v>-4.62</v>
-      </c>
-      <c r="I23" s="2" t="n">
-        <v>-31.85</v>
+        <v>411.41</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>18.51</v>
       </c>
       <c r="J23" t="n">
-        <v>-134.86</v>
+        <v>147.38</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner S9 SE</t>
+          <t>BITMAIN AntMiner T17+</t>
         </is>
       </c>
       <c r="B24" s="1" t="n">
-        <v>4.18</v>
+        <v>19.83</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>29.76</v>
+        <v>139.44</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>129.17</v>
+        <v>679.86</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>8.6</v>
+        <v>19.97</v>
       </c>
       <c r="F24" s="1" t="n">
-        <v>60.21</v>
+        <v>139.78</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>258.05</v>
+        <v>598.42</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>-4.42</v>
+        <v>-0.14</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>-30.45</v>
+        <v>-0.34</v>
       </c>
       <c r="J24" t="n">
-        <v>-128.88</v>
+        <v>81.45</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner T15</t>
+          <t>BITMAIN AntMiner T17e</t>
         </is>
       </c>
       <c r="B25" s="1" t="n">
-        <v>5.83</v>
+        <v>14.39</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>42.04</v>
+        <v>100.91</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>176.43</v>
+        <v>490.03</v>
       </c>
       <c r="E25" s="1" t="n">
-        <v>10.24</v>
+        <v>18.19</v>
       </c>
       <c r="F25" s="1" t="n">
-        <v>72.33</v>
+        <v>127.33</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>310.36</v>
+        <v>545.12</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>-4.41</v>
+        <v>-3.8</v>
       </c>
       <c r="I25" s="2" t="n">
-        <v>-30.29</v>
+        <v>-26.42</v>
       </c>
       <c r="J25" t="n">
-        <v>-133.93</v>
+        <v>-55.09</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner T17</t>
+          <t>BITMAIN AntMiner T9+</t>
         </is>
       </c>
       <c r="B26" s="1" t="n">
-        <v>15.69</v>
+        <v>2.85</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>111.65</v>
+        <v>20.06</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>484.63</v>
+        <v>97.79000000000001</v>
       </c>
       <c r="E26" s="1" t="n">
-        <v>14.78</v>
+        <v>8.94</v>
       </c>
       <c r="F26" s="1" t="n">
-        <v>103.49</v>
+        <v>62.55</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>443.52</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="I26" s="1" t="n">
-        <v>8.16</v>
+        <v>267.79</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>-6.08</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>-42.49</v>
       </c>
       <c r="J26" t="n">
-        <v>41.11</v>
+        <v>-170</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner T17+</t>
+          <t>BITMAIN AntMiner Z11</t>
         </is>
       </c>
       <c r="B27" s="1" t="n">
-        <v>19.09</v>
+        <v>18.64</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>135.84</v>
+        <v>135.46</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>589.63</v>
+        <v>549.13</v>
       </c>
       <c r="E27" s="1" t="n">
-        <v>21.5</v>
+        <v>8.85</v>
       </c>
       <c r="F27" s="1" t="n">
-        <v>150.53</v>
+        <v>61.94</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>645.12</v>
-      </c>
-      <c r="H27" s="2" t="n">
-        <v>-2.41</v>
-      </c>
-      <c r="I27" s="2" t="n">
-        <v>-14.69</v>
+        <v>265.17</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <v>9.789999999999999</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>73.52</v>
       </c>
       <c r="J27" t="n">
-        <v>-55.49</v>
+        <v>283.96</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner T17e</t>
+          <t>Baikal BK-G28</t>
         </is>
       </c>
       <c r="B28" s="1" t="n">
-        <v>13.58</v>
+        <v>5.87</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>97.03</v>
+        <v>40.11</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>406.7</v>
+        <v>228.01</v>
       </c>
       <c r="E28" s="1" t="n">
-        <v>19.59</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="F28" s="1" t="n">
-        <v>137.12</v>
+        <v>56.78</v>
       </c>
       <c r="G28" s="1" t="n">
-        <v>587.66</v>
+        <v>243.11</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>-6.01</v>
+        <v>-2.24</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>-40.09</v>
+        <v>-16.67</v>
       </c>
       <c r="J28" t="n">
-        <v>-180.96</v>
+        <v>-15.1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner T9+</t>
+          <t>Baikal Giant X10</t>
         </is>
       </c>
       <c r="B29" s="1" t="n">
-        <v>2.75</v>
+        <v>2.1</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>19.54</v>
+        <v>14.33</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>84.81</v>
+        <v>81.43000000000001</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>9.619999999999999</v>
+        <v>4.06</v>
       </c>
       <c r="F29" s="1" t="n">
-        <v>67.36</v>
+        <v>28.39</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>288.69</v>
+        <v>121.55</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>-6.88</v>
+        <v>-1.96</v>
       </c>
       <c r="I29" s="2" t="n">
-        <v>-47.82</v>
+        <v>-14.07</v>
       </c>
       <c r="J29" t="n">
-        <v>-203.88</v>
+        <v>-40.12</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BITMAIN AntMiner Z11</t>
+          <t>Baikal Giant+</t>
         </is>
       </c>
       <c r="B30" s="1" t="n">
-        <v>4.67</v>
+        <v>1.12</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>33.11</v>
+        <v>9.32</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>188.37</v>
+        <v>27.03</v>
       </c>
       <c r="E30" s="1" t="n">
-        <v>9.529999999999999</v>
+        <v>2.68</v>
       </c>
       <c r="F30" s="1" t="n">
-        <v>66.7</v>
+        <v>18.78</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>285.87</v>
+        <v>80.41</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>-4.86</v>
+        <v>-1.56</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>-33.6</v>
+        <v>-9.460000000000001</v>
       </c>
       <c r="J30" t="n">
-        <v>-97.5</v>
+        <v>-53.39</v>
       </c>
     </row>
     <row r="31">
@@ -1478,31 +1478,31 @@
         </is>
       </c>
       <c r="B31" s="1" t="n">
-        <v>9.68</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>68.83</v>
+        <v>70.33</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>298.71</v>
+        <v>342.95</v>
       </c>
       <c r="E31" s="1" t="n">
-        <v>15.99</v>
+        <v>14.85</v>
       </c>
       <c r="F31" s="1" t="n">
-        <v>111.96</v>
+        <v>103.96</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>479.81</v>
+        <v>445.07</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>-6.32</v>
+        <v>-4.97</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>-43.13</v>
+        <v>-33.63</v>
       </c>
       <c r="J31" t="n">
-        <v>-181.1</v>
+        <v>-102.12</v>
       </c>
     </row>
     <row r="32">
@@ -1512,31 +1512,31 @@
         </is>
       </c>
       <c r="B32" s="1" t="n">
-        <v>13.08</v>
+        <v>13.35</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>93.01000000000001</v>
+        <v>95.03</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>403.66</v>
+        <v>463.45</v>
       </c>
       <c r="E32" s="1" t="n">
-        <v>21.84</v>
+        <v>20.28</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>152.88</v>
+        <v>141.96</v>
       </c>
       <c r="G32" s="1" t="n">
-        <v>655.2</v>
+        <v>607.77</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>-8.76</v>
+        <v>-6.93</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>-59.87</v>
+        <v>-46.93</v>
       </c>
       <c r="J32" t="n">
-        <v>-251.54</v>
+        <v>-144.32</v>
       </c>
     </row>
     <row r="33">
@@ -1546,31 +1546,31 @@
         </is>
       </c>
       <c r="B33" s="1" t="n">
-        <v>1.91</v>
+        <v>1.95</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>13.58</v>
+        <v>13.88</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>58.93</v>
+        <v>67.66</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>7.73</v>
+        <v>7.18</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>54.1</v>
+        <v>50.23</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>231.84</v>
+        <v>215.06</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>-5.82</v>
+        <v>-5.23</v>
       </c>
       <c r="I33" s="2" t="n">
-        <v>-40.52</v>
+        <v>-36.36</v>
       </c>
       <c r="J33" t="n">
-        <v>-172.91</v>
+        <v>-147.39</v>
       </c>
     </row>
     <row r="34">
@@ -1580,31 +1580,31 @@
         </is>
       </c>
       <c r="B34" s="1" t="n">
-        <v>5.23</v>
+        <v>5.34</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>37.21</v>
+        <v>38.01</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>161.46</v>
+        <v>185.38</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>11.42</v>
+        <v>10.61</v>
       </c>
       <c r="F34" s="1" t="n">
-        <v>79.97</v>
+        <v>74.26000000000001</v>
       </c>
       <c r="G34" s="1" t="n">
-        <v>342.72</v>
+        <v>317.91</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>-6.19</v>
+        <v>-5.27</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>-42.76</v>
+        <v>-36.24</v>
       </c>
       <c r="J34" t="n">
-        <v>-181.26</v>
+        <v>-132.53</v>
       </c>
     </row>
     <row r="35">
@@ -1614,31 +1614,31 @@
         </is>
       </c>
       <c r="B35" s="1" t="n">
-        <v>1.21</v>
+        <v>1.68</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>9.539999999999999</v>
+        <v>11.67</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>56.4</v>
+        <v>51.81</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>8.06</v>
+        <v>7.49</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>56.45</v>
+        <v>52.42</v>
       </c>
       <c r="G35" s="1" t="n">
-        <v>241.92</v>
+        <v>224.41</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>-6.86</v>
+        <v>-5.81</v>
       </c>
       <c r="I35" s="2" t="n">
-        <v>-46.91</v>
+        <v>-40.75</v>
       </c>
       <c r="J35" t="n">
-        <v>-185.52</v>
+        <v>-172.59</v>
       </c>
     </row>
     <row r="36">
@@ -1648,31 +1648,31 @@
         </is>
       </c>
       <c r="B36" s="1" t="n">
-        <v>11.51</v>
+        <v>11.75</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>81.84999999999999</v>
+        <v>83.63</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>355.22</v>
+        <v>407.84</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>16.8</v>
+        <v>15.6</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>117.6</v>
+        <v>109.2</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>504</v>
+        <v>467.51</v>
       </c>
       <c r="H36" s="2" t="n">
-        <v>-5.29</v>
+        <v>-3.85</v>
       </c>
       <c r="I36" s="2" t="n">
-        <v>-35.75</v>
+        <v>-25.57</v>
       </c>
       <c r="J36" t="n">
-        <v>-148.78</v>
+        <v>-59.68</v>
       </c>
     </row>
     <row r="37">
@@ -1682,31 +1682,31 @@
         </is>
       </c>
       <c r="B37" s="1" t="n">
-        <v>13.08</v>
+        <v>13.35</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>93.01000000000001</v>
+        <v>95.01000000000001</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>403.66</v>
+        <v>463.42</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>16.8</v>
+        <v>15.6</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>117.6</v>
+        <v>109.2</v>
       </c>
       <c r="G37" s="1" t="n">
-        <v>504</v>
+        <v>467.51</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>-3.72</v>
+        <v>-2.25</v>
       </c>
       <c r="I37" s="2" t="n">
-        <v>-24.59</v>
+        <v>-14.19</v>
       </c>
       <c r="J37" t="n">
-        <v>-100.34</v>
+        <v>-4.09</v>
       </c>
     </row>
     <row r="38">
@@ -1716,31 +1716,31 @@
         </is>
       </c>
       <c r="B38" s="1" t="n">
-        <v>2.3</v>
+        <v>3.18</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>18.18</v>
+        <v>22.21</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>107.49</v>
+        <v>98.69</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>7.46</v>
+        <v>6.85</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>52.21</v>
+        <v>48.41</v>
       </c>
       <c r="G38" s="1" t="n">
-        <v>223.78</v>
+        <v>207.5</v>
       </c>
       <c r="H38" s="2" t="n">
-        <v>-5.16</v>
+        <v>-3.68</v>
       </c>
       <c r="I38" s="2" t="n">
-        <v>-34.03</v>
+        <v>-26.2</v>
       </c>
       <c r="J38" t="n">
-        <v>-116.28</v>
+        <v>-108.81</v>
       </c>
     </row>
     <row r="39">
@@ -1750,31 +1750,31 @@
         </is>
       </c>
       <c r="B39" s="1" t="n">
-        <v>4.11</v>
+        <v>2.9</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>25.61</v>
+        <v>23.41</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>138.29</v>
+        <v>106.53</v>
       </c>
       <c r="E39" s="1" t="n">
-        <v>6.38</v>
+        <v>5.87</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>44.69</v>
+        <v>41.43</v>
       </c>
       <c r="G39" s="1" t="n">
-        <v>191.52</v>
+        <v>177.59</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>-2.28</v>
+        <v>-2.96</v>
       </c>
       <c r="I39" s="2" t="n">
-        <v>-19.08</v>
+        <v>-18.02</v>
       </c>
       <c r="J39" t="n">
-        <v>-53.23</v>
+        <v>-71.06</v>
       </c>
     </row>
     <row r="40">
@@ -1784,235 +1784,235 @@
         </is>
       </c>
       <c r="B40" s="1" t="n">
-        <v>4.85</v>
+        <v>9.449999999999999</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>34.8</v>
+        <v>78.86</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>170.95</v>
+        <v>299.24</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>9.539999999999999</v>
+        <v>8.77</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>66.8</v>
+        <v>61.93</v>
       </c>
       <c r="G40" s="1" t="n">
-        <v>286.27</v>
-      </c>
-      <c r="H40" s="2" t="n">
-        <v>-4.69</v>
-      </c>
-      <c r="I40" s="2" t="n">
-        <v>-31.99</v>
+        <v>265.45</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>16.93</v>
       </c>
       <c r="J40" t="n">
-        <v>-115.32</v>
+        <v>33.78</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>iBeLink DM22G X11</t>
+          <t>Innosilicon A4 Dominator</t>
         </is>
       </c>
       <c r="B41" s="1" t="n">
-        <v>0.41</v>
+        <v>6.85</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>2.92</v>
+        <v>46.56</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>14.35</v>
+        <v>160.97</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>5.44</v>
+        <v>6.48</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>38.1</v>
+        <v>45.8</v>
       </c>
       <c r="G41" s="1" t="n">
-        <v>163.3</v>
-      </c>
-      <c r="H41" s="2" t="n">
-        <v>-5.04</v>
-      </c>
-      <c r="I41" s="2" t="n">
-        <v>-35.18</v>
+        <v>196.29</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>0.77</v>
       </c>
       <c r="J41" t="n">
-        <v>-148.94</v>
+        <v>-35.31</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Innosilicon A4 Dominator</t>
+          <t>Innosilicon A5</t>
         </is>
       </c>
       <c r="B42" s="1" t="n">
-        <v>1.44</v>
+        <v>2.34</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>10.33</v>
+        <v>19.57</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>43.66</v>
+        <v>74.23999999999999</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>7.06</v>
+        <v>9.26</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>49.39</v>
+        <v>65.42</v>
       </c>
       <c r="G42" s="1" t="n">
-        <v>211.68</v>
+        <v>280.41</v>
       </c>
       <c r="H42" s="2" t="n">
-        <v>-5.62</v>
+        <v>-6.92</v>
       </c>
       <c r="I42" s="2" t="n">
-        <v>-39.07</v>
+        <v>-45.86</v>
       </c>
       <c r="J42" t="n">
-        <v>-168.02</v>
+        <v>-206.17</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Innosilicon A5</t>
+          <t>Innosilicon A5 DashMaster - normal mode</t>
         </is>
       </c>
       <c r="B43" s="1" t="n">
-        <v>1.2</v>
+        <v>1.09</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>8.630000000000001</v>
+        <v>9.09</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>42.41</v>
+        <v>34.49</v>
       </c>
       <c r="E43" s="1" t="n">
-        <v>10.08</v>
+        <v>4.63</v>
       </c>
       <c r="F43" s="1" t="n">
-        <v>70.56</v>
+        <v>32.71</v>
       </c>
       <c r="G43" s="1" t="n">
-        <v>302.4</v>
+        <v>140.2</v>
       </c>
       <c r="H43" s="2" t="n">
-        <v>-8.880000000000001</v>
+        <v>-3.54</v>
       </c>
       <c r="I43" s="2" t="n">
-        <v>-61.93</v>
+        <v>-23.62</v>
       </c>
       <c r="J43" t="n">
-        <v>-259.99</v>
+        <v>-105.71</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Innosilicon A5 DashMaster - normal mode</t>
+          <t>Innosilicon A5 DashMaster - overclock mode</t>
         </is>
       </c>
       <c r="B44" s="1" t="n">
-        <v>0.5600000000000001</v>
+        <v>1.37</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>4.01</v>
+        <v>11.44</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>19.7</v>
+        <v>43.4</v>
       </c>
       <c r="E44" s="1" t="n">
-        <v>5.04</v>
+        <v>7.72</v>
       </c>
       <c r="F44" s="1" t="n">
-        <v>35.28</v>
+        <v>54.52</v>
       </c>
       <c r="G44" s="1" t="n">
-        <v>151.2</v>
+        <v>233.68</v>
       </c>
       <c r="H44" s="2" t="n">
-        <v>-4.48</v>
+        <v>-6.35</v>
       </c>
       <c r="I44" s="2" t="n">
-        <v>-31.27</v>
+        <v>-43.08</v>
       </c>
       <c r="J44" t="n">
-        <v>-131.5</v>
+        <v>-190.27</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Innosilicon A5 DashMaster - overclock mode</t>
+          <t>Innosilicon A6</t>
         </is>
       </c>
       <c r="B45" s="1" t="n">
-        <v>0.7</v>
+        <v>30.1</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>5.05</v>
+        <v>204.55</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>24.79</v>
+        <v>707.13</v>
       </c>
       <c r="E45" s="1" t="n">
-        <v>8.4</v>
+        <v>9.26</v>
       </c>
       <c r="F45" s="1" t="n">
-        <v>58.8</v>
+        <v>65.42</v>
       </c>
       <c r="G45" s="1" t="n">
-        <v>252</v>
-      </c>
-      <c r="H45" s="2" t="n">
-        <v>-7.7</v>
-      </c>
-      <c r="I45" s="2" t="n">
-        <v>-53.75</v>
+        <v>280.41</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <v>20.84</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>139.13</v>
       </c>
       <c r="J45" t="n">
-        <v>-227.21</v>
+        <v>426.72</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Innosilicon A6</t>
+          <t>Innosilicon A9 ZMaster</t>
         </is>
       </c>
       <c r="B46" s="1" t="n">
-        <v>6.31</v>
+        <v>6.83</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>45.36</v>
+        <v>50.07</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>191.81</v>
+        <v>203.32</v>
       </c>
       <c r="E46" s="1" t="n">
-        <v>10.08</v>
+        <v>3.83</v>
       </c>
       <c r="F46" s="1" t="n">
-        <v>70.56</v>
+        <v>27.04</v>
       </c>
       <c r="G46" s="1" t="n">
-        <v>302.4</v>
-      </c>
-      <c r="H46" s="2" t="n">
-        <v>-3.77</v>
-      </c>
-      <c r="I46" s="2" t="n">
-        <v>-25.2</v>
+        <v>115.9</v>
+      </c>
+      <c r="H46" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>23.02</v>
       </c>
       <c r="J46" t="n">
-        <v>-110.59</v>
+        <v>87.42</v>
       </c>
     </row>
     <row r="47">
@@ -2022,167 +2022,167 @@
         </is>
       </c>
       <c r="B47" s="1" t="n">
-        <v>4.15</v>
+        <v>16.39</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>29.43</v>
+        <v>120.16</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>167.44</v>
+        <v>487.98</v>
       </c>
       <c r="E47" s="1" t="n">
-        <v>10.42</v>
+        <v>9.57</v>
       </c>
       <c r="F47" s="1" t="n">
-        <v>72.91</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="G47" s="1" t="n">
-        <v>312.48</v>
-      </c>
-      <c r="H47" s="2" t="n">
-        <v>-6.27</v>
-      </c>
-      <c r="I47" s="2" t="n">
-        <v>-43.48</v>
+        <v>289.76</v>
+      </c>
+      <c r="H47" s="1" t="n">
+        <v>6.82</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>52.56</v>
       </c>
       <c r="J47" t="n">
-        <v>-145.04</v>
+        <v>198.22</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Innosilicon A9 ZMaster</t>
+          <t>Innosilicon D9+</t>
         </is>
       </c>
       <c r="B48" s="1" t="n">
-        <v>1.73</v>
+        <v>3.03</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>12.26</v>
+        <v>20.71</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>69.77</v>
+        <v>69</v>
       </c>
       <c r="E48" s="1" t="n">
-        <v>4.17</v>
+        <v>7.68</v>
       </c>
       <c r="F48" s="1" t="n">
-        <v>29.16</v>
+        <v>53.73</v>
       </c>
       <c r="G48" s="1" t="n">
-        <v>124.99</v>
+        <v>230.02</v>
       </c>
       <c r="H48" s="2" t="n">
-        <v>-2.44</v>
+        <v>-4.65</v>
       </c>
       <c r="I48" s="2" t="n">
-        <v>-16.9</v>
+        <v>-33.02</v>
       </c>
       <c r="J48" t="n">
-        <v>-55.22</v>
+        <v>-161.02</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Innosilicon D9+</t>
+          <t>Innosilicon T3 50T</t>
         </is>
       </c>
       <c r="B49" s="1" t="n">
-        <v>0.02</v>
+        <v>13.21</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>0.9399999999999999</v>
+        <v>94.84999999999999</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>7.27</v>
+        <v>463.25</v>
       </c>
       <c r="E49" s="1" t="n">
-        <v>8.27</v>
+        <v>19.14</v>
       </c>
       <c r="F49" s="1" t="n">
-        <v>57.86</v>
+        <v>135.21</v>
       </c>
       <c r="G49" s="1" t="n">
-        <v>247.97</v>
+        <v>579.51</v>
       </c>
       <c r="H49" s="2" t="n">
-        <v>-8.25</v>
+        <v>-5.93</v>
       </c>
       <c r="I49" s="2" t="n">
-        <v>-56.92</v>
+        <v>-40.36</v>
       </c>
       <c r="J49" t="n">
-        <v>-240.7</v>
+        <v>-116.26</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Innosilicon T2</t>
+          <t>Innosilicon T3+ 52T</t>
         </is>
       </c>
       <c r="B50" s="1" t="n">
-        <v>4.45</v>
+        <v>13.74</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>31.63</v>
+        <v>98.64</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>137.31</v>
+        <v>481.78</v>
       </c>
       <c r="E50" s="1" t="n">
-        <v>10.62</v>
+        <v>17.29</v>
       </c>
       <c r="F50" s="1" t="n">
-        <v>74.31999999999999</v>
+        <v>122.12</v>
       </c>
       <c r="G50" s="1" t="n">
-        <v>318.53</v>
+        <v>523.4299999999999</v>
       </c>
       <c r="H50" s="2" t="n">
-        <v>-6.17</v>
+        <v>-3.55</v>
       </c>
       <c r="I50" s="2" t="n">
-        <v>-42.69</v>
+        <v>-23.48</v>
       </c>
       <c r="J50" t="n">
-        <v>-181.22</v>
+        <v>-41.65</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Innosilicon T2-26T</t>
+          <t>Innosilicon T3+ 57T</t>
         </is>
       </c>
       <c r="B51" s="1" t="n">
-        <v>6.8</v>
+        <v>15.06</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>48.38</v>
+        <v>108.13</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>210</v>
+        <v>528.11</v>
       </c>
       <c r="E51" s="1" t="n">
-        <v>14.11</v>
+        <v>20.38</v>
       </c>
       <c r="F51" s="1" t="n">
-        <v>98.78</v>
+        <v>143.93</v>
       </c>
       <c r="G51" s="1" t="n">
-        <v>423.36</v>
+        <v>616.9</v>
       </c>
       <c r="H51" s="2" t="n">
-        <v>-7.31</v>
+        <v>-5.31</v>
       </c>
       <c r="I51" s="2" t="n">
-        <v>-50.4</v>
+        <v>-35.8</v>
       </c>
       <c r="J51" t="n">
-        <v>-213.36</v>
+        <v>-88.79000000000001</v>
       </c>
     </row>
     <row r="52">
@@ -2192,31 +2192,31 @@
         </is>
       </c>
       <c r="B52" s="1" t="n">
-        <v>10.09</v>
+        <v>10.48</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>72.45999999999999</v>
+        <v>74.34999999999999</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>314.89</v>
+        <v>363.06</v>
       </c>
       <c r="E52" s="1" t="n">
-        <v>14.3</v>
+        <v>13.28</v>
       </c>
       <c r="F52" s="1" t="n">
-        <v>100.99</v>
+        <v>93.77</v>
       </c>
       <c r="G52" s="1" t="n">
-        <v>433.29</v>
+        <v>401.92</v>
       </c>
       <c r="H52" s="2" t="n">
-        <v>-4.2</v>
+        <v>-2.79</v>
       </c>
       <c r="I52" s="2" t="n">
-        <v>-28.53</v>
+        <v>-19.42</v>
       </c>
       <c r="J52" t="n">
-        <v>-118.4</v>
+        <v>-38.86</v>
       </c>
     </row>
     <row r="53">
@@ -2226,371 +2226,235 @@
         </is>
       </c>
       <c r="B53" s="1" t="n">
-        <v>11.13</v>
+        <v>11.56</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>79.89</v>
+        <v>81.97</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>347.19</v>
+        <v>400.3</v>
       </c>
       <c r="E53" s="1" t="n">
-        <v>13.97</v>
+        <v>12.97</v>
       </c>
       <c r="F53" s="1" t="n">
-        <v>98.64</v>
+        <v>91.59</v>
       </c>
       <c r="G53" s="1" t="n">
-        <v>423.21</v>
+        <v>392.57</v>
       </c>
       <c r="H53" s="2" t="n">
-        <v>-2.84</v>
+        <v>-1.41</v>
       </c>
       <c r="I53" s="2" t="n">
-        <v>-18.75</v>
+        <v>-9.619999999999999</v>
       </c>
       <c r="J53" t="n">
-        <v>-76.03</v>
+        <v>7.72</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Innosilicon T3 50T</t>
+          <t>MicroBT Whatsminer M10</t>
         </is>
       </c>
       <c r="B54" s="1" t="n">
-        <v>12.94</v>
+        <v>8.960000000000001</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>92.87</v>
+        <v>63</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>403.51</v>
+        <v>307.3</v>
       </c>
       <c r="E54" s="1" t="n">
-        <v>20.61</v>
+        <v>13.38</v>
       </c>
       <c r="F54" s="1" t="n">
-        <v>145.61</v>
+        <v>93.69</v>
       </c>
       <c r="G54" s="1" t="n">
-        <v>624.74</v>
+        <v>401.13</v>
       </c>
       <c r="H54" s="2" t="n">
-        <v>-7.68</v>
+        <v>-4.43</v>
       </c>
       <c r="I54" s="2" t="n">
-        <v>-52.74</v>
+        <v>-30.69</v>
       </c>
       <c r="J54" t="n">
-        <v>-221.23</v>
+        <v>-93.83</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Innosilicon T3+ 52T</t>
+          <t>MicroBT Whatsminer M10S</t>
         </is>
       </c>
       <c r="B55" s="1" t="n">
-        <v>13.46</v>
+        <v>14.93</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>96.59</v>
+        <v>105</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>419.65</v>
+        <v>512.16</v>
       </c>
       <c r="E55" s="1" t="n">
-        <v>18.62</v>
+        <v>21.84</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>131.52</v>
+        <v>152.88</v>
       </c>
       <c r="G55" s="1" t="n">
-        <v>564.28</v>
+        <v>654.52</v>
       </c>
       <c r="H55" s="2" t="n">
-        <v>-5.16</v>
+        <v>-6.91</v>
       </c>
       <c r="I55" s="2" t="n">
-        <v>-34.93</v>
+        <v>-47.88</v>
       </c>
       <c r="J55" t="n">
-        <v>-144.63</v>
+        <v>-142.36</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Innosilicon T3+ 57T</t>
+          <t>MicroBT Whatsminer M20S</t>
         </is>
       </c>
       <c r="B56" s="1" t="n">
-        <v>14.75</v>
+        <v>18.27</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>105.87</v>
+        <v>129.21</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>460.01</v>
+        <v>628.45</v>
       </c>
       <c r="E56" s="1" t="n">
-        <v>21.95</v>
+        <v>20.75</v>
       </c>
       <c r="F56" s="1" t="n">
-        <v>155</v>
+        <v>146.55</v>
       </c>
       <c r="G56" s="1" t="n">
-        <v>665.05</v>
+        <v>628.12</v>
       </c>
       <c r="H56" s="2" t="n">
-        <v>-7.19</v>
+        <v>-2.48</v>
       </c>
       <c r="I56" s="2" t="n">
-        <v>-49.13</v>
+        <v>-17.34</v>
       </c>
       <c r="J56" t="n">
-        <v>-205.04</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>MicroBT Whatsminer M10</t>
+          <t>MicroBT Whatsminer M21S</t>
         </is>
       </c>
       <c r="B57" s="1" t="n">
-        <v>8.539999999999999</v>
+        <v>15.2</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>61.31</v>
+        <v>106.56</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>266.45</v>
+        <v>517.7</v>
       </c>
       <c r="E57" s="1" t="n">
-        <v>14.26</v>
+        <v>20.97</v>
       </c>
       <c r="F57" s="1" t="n">
-        <v>100.75</v>
+        <v>146.76</v>
       </c>
       <c r="G57" s="1" t="n">
-        <v>432.28</v>
+        <v>628.34</v>
       </c>
       <c r="H57" s="2" t="n">
-        <v>-5.72</v>
+        <v>-5.77</v>
       </c>
       <c r="I57" s="2" t="n">
-        <v>-39.44</v>
+        <v>-40.2</v>
       </c>
       <c r="J57" t="n">
-        <v>-165.84</v>
+        <v>-110.64</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>MicroBT Whatsminer M10S</t>
+          <t>MicroBT Whatsminer M30S</t>
         </is>
       </c>
       <c r="B58" s="1" t="n">
-        <v>14.23</v>
+        <v>23.35</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>102.19</v>
+        <v>164.18</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>444.08</v>
+        <v>800.83</v>
       </c>
       <c r="E58" s="1" t="n">
-        <v>23.28</v>
+        <v>20.39</v>
       </c>
       <c r="F58" s="1" t="n">
-        <v>164.4</v>
+        <v>142.75</v>
       </c>
       <c r="G58" s="1" t="n">
-        <v>705.36</v>
-      </c>
-      <c r="H58" s="2" t="n">
-        <v>-9.039999999999999</v>
-      </c>
-      <c r="I58" s="2" t="n">
-        <v>-62.21</v>
+        <v>611.13</v>
+      </c>
+      <c r="H58" s="1" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="I58" s="1" t="n">
+        <v>21.44</v>
       </c>
       <c r="J58" t="n">
-        <v>-261.28</v>
+        <v>189.7</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>MicroBT Whatsminer M20S</t>
-        </is>
-      </c>
-      <c r="B59" s="1" t="n">
-        <v>17.24</v>
-      </c>
-      <c r="C59" s="1" t="n">
-        <v>124.3</v>
-      </c>
-      <c r="D59" s="1" t="n">
-        <v>521.63</v>
-      </c>
-      <c r="E59" s="1" t="n">
-        <v>22.34</v>
-      </c>
-      <c r="F59" s="1" t="n">
-        <v>157.82</v>
-      </c>
-      <c r="G59" s="1" t="n">
-        <v>677.14</v>
-      </c>
-      <c r="H59" s="2" t="n">
-        <v>-5.1</v>
-      </c>
-      <c r="I59" s="2" t="n">
-        <v>-33.52</v>
+          <t>MicroBT Whatsminer M31S</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>18.81</v>
+      </c>
+      <c r="C59" t="n">
+        <v>133.45</v>
+      </c>
+      <c r="D59" t="n">
+        <v>651.65</v>
+      </c>
+      <c r="E59" t="n">
+        <v>19.88</v>
+      </c>
+      <c r="F59" t="n">
+        <v>140.44</v>
+      </c>
+      <c r="G59" t="n">
+        <v>601.95</v>
+      </c>
+      <c r="H59" t="n">
+        <v>-1.07</v>
+      </c>
+      <c r="I59" t="n">
+        <v>-6.99</v>
       </c>
       <c r="J59" t="n">
-        <v>-155.51</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>MicroBT Whatsminer M21S</t>
-        </is>
-      </c>
-      <c r="B60" s="1" t="n">
-        <v>14.2</v>
-      </c>
-      <c r="C60" s="1" t="n">
-        <v>102.36</v>
-      </c>
-      <c r="D60" s="1" t="n">
-        <v>429.58</v>
-      </c>
-      <c r="E60" s="1" t="n">
-        <v>22.34</v>
-      </c>
-      <c r="F60" s="1" t="n">
-        <v>157.82</v>
-      </c>
-      <c r="G60" s="1" t="n">
-        <v>677.14</v>
-      </c>
-      <c r="H60" s="2" t="n">
-        <v>-8.140000000000001</v>
-      </c>
-      <c r="I60" s="2" t="n">
-        <v>-55.46</v>
-      </c>
-      <c r="J60" t="n">
-        <v>-247.56</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>MicroBT Whatsminer M30S</t>
-        </is>
-      </c>
-      <c r="B61" s="1" t="n">
-        <v>22.26</v>
-      </c>
-      <c r="C61" s="1" t="n">
-        <v>159.78</v>
-      </c>
-      <c r="D61" s="1" t="n">
-        <v>694.37</v>
-      </c>
-      <c r="E61" s="1" t="n">
-        <v>21.73</v>
-      </c>
-      <c r="F61" s="1" t="n">
-        <v>153.5</v>
-      </c>
-      <c r="G61" s="1" t="n">
-        <v>658.6</v>
-      </c>
-      <c r="H61" s="1" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="I61" s="1" t="n">
-        <v>6.28</v>
-      </c>
-      <c r="J61" t="n">
-        <v>35.77</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>MicroBT Whatsminer M31S</t>
-        </is>
-      </c>
-      <c r="B62" s="1" t="n">
-        <v>18.12</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <v>130.06</v>
-      </c>
-      <c r="D62" s="1" t="n">
-        <v>565.1900000000001</v>
-      </c>
-      <c r="E62" s="1" t="n">
-        <v>21.41</v>
-      </c>
-      <c r="F62" s="1" t="n">
-        <v>151.24</v>
-      </c>
-      <c r="G62" s="1" t="n">
-        <v>648.9299999999999</v>
-      </c>
-      <c r="H62" s="2" t="n">
-        <v>-3.3</v>
-      </c>
-      <c r="I62" s="2" t="n">
-        <v>-21.19</v>
-      </c>
-      <c r="J62" t="n">
-        <v>-83.73999999999999</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>StrongU STU-U6</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>8.06</v>
-      </c>
-      <c r="C63" t="n">
-        <v>58.32</v>
-      </c>
-      <c r="D63" t="n">
-        <v>286.98</v>
-      </c>
-      <c r="E63" t="n">
-        <v>14.63</v>
-      </c>
-      <c r="F63" t="n">
-        <v>103.33</v>
-      </c>
-      <c r="G63" t="n">
-        <v>443.37</v>
-      </c>
-      <c r="H63" t="n">
-        <v>-6.57</v>
-      </c>
-      <c r="I63" t="n">
-        <v>-45.01</v>
-      </c>
-      <c r="J63" t="n">
-        <v>-156.38</v>
+        <v>49.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>